<commit_message>
Erica adds cover into Isla's phd relationship
</commit_message>
<xml_diff>
--- a/data/allometry/Isla_phd/Percent_cover_Pika.xlsx
+++ b/data/allometry/Isla_phd/Percent_cover_Pika.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericazaja/Desktop/Github_repos.tmp/NEW_MSC_ZAJA_2022/data/allometry/Isla_phd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C10E32C-654A-1840-A1C5-CF1538440AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74B30AF-D6F1-E045-AB46-F804FA9DBF40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="960" windowWidth="27640" windowHeight="15680" xr2:uid="{A59DA1AF-F7B0-3A40-B4D4-1BD9347FEB4C}"/>
   </bookViews>
@@ -279,7 +279,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -289,6 +289,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -305,12 +311,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,14 +635,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D2DD77-D489-504A-94E8-ADECF01E707A}">
   <dimension ref="A1:AB51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="265" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" topLeftCell="E18" zoomScale="233" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.1640625" style="2"/>
-    <col min="2" max="27" width="9.1640625" style="1"/>
+    <col min="2" max="9" width="9.1640625" style="1"/>
+    <col min="10" max="10" width="9.1640625" style="5"/>
+    <col min="11" max="27" width="9.1640625" style="1"/>
     <col min="28" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
@@ -666,7 +676,7 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -746,7 +756,7 @@
       <c r="I2" s="3">
         <v>0</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="6">
         <v>7.0519054101980352</v>
       </c>
       <c r="K2" s="3">
@@ -826,7 +836,7 @@
       <c r="I3" s="3">
         <v>0</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="6">
         <v>27.344942163609716</v>
       </c>
       <c r="K3" s="3">
@@ -906,7 +916,7 @@
       <c r="I4" s="3">
         <v>0</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="6">
         <v>36.106139934387627</v>
       </c>
       <c r="K4" s="3">
@@ -966,7 +976,7 @@
       <c r="I5" s="3">
         <v>0</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="6">
         <v>49.777147140102649</v>
       </c>
       <c r="K5" s="3">
@@ -1023,7 +1033,7 @@
       <c r="I6" s="3">
         <v>0</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="6">
         <v>52.838382278972716</v>
       </c>
       <c r="K6" s="3">
@@ -1103,7 +1113,7 @@
       <c r="I7" s="3">
         <v>0</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="6">
         <v>57.143359888792602</v>
       </c>
       <c r="K7" s="3">
@@ -1195,7 +1205,7 @@
       <c r="I8" s="3">
         <v>0</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="6">
         <v>58.665247684869414</v>
       </c>
       <c r="K8" s="3">
@@ -1239,7 +1249,7 @@
       <c r="I9" s="3">
         <v>0</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="6">
         <v>65.335800870830496</v>
       </c>
       <c r="K9" s="3">
@@ -1326,7 +1336,7 @@
       <c r="I10" s="3">
         <v>0</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="6">
         <v>66.025481709347204</v>
       </c>
       <c r="K10" s="3">
@@ -1370,7 +1380,7 @@
       <c r="I11" s="3">
         <v>0</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="6">
         <v>66.399414156759235</v>
       </c>
       <c r="K11" s="3">
@@ -1414,7 +1424,7 @@
       <c r="I12" s="3">
         <v>0</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="6">
         <v>72.455373819027344</v>
       </c>
       <c r="K12" s="3">
@@ -1458,7 +1468,7 @@
       <c r="I13" s="3">
         <v>0</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="6">
         <v>76.867916144392936</v>
       </c>
       <c r="K13" s="3">
@@ -1502,7 +1512,7 @@
       <c r="I14" s="3">
         <v>0</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="6">
         <v>81.727268902044841</v>
       </c>
       <c r="K14" s="3">
@@ -1546,7 +1556,7 @@
       <c r="I15" s="3">
         <v>0.32779517296139266</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="6">
         <v>35.856716954561122</v>
       </c>
       <c r="K15" s="3">
@@ -1590,7 +1600,7 @@
       <c r="I16" s="3">
         <v>0.72817141627063653</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="6">
         <v>20.215967611067882</v>
       </c>
       <c r="K16" s="3">
@@ -1634,7 +1644,7 @@
       <c r="I17" s="3">
         <v>4.7342444422817582</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="6">
         <v>19.010941649172075</v>
       </c>
       <c r="K17" s="3">
@@ -1678,7 +1688,7 @@
       <c r="I18" s="3">
         <v>7.0778135644480153</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="6">
         <v>46.411313199100206</v>
       </c>
       <c r="K18" s="3">
@@ -1722,7 +1732,7 @@
       <c r="I19" s="3">
         <v>9.5772776122236554</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="6">
         <v>8.440887008465296</v>
       </c>
       <c r="K19" s="3">
@@ -1766,7 +1776,7 @@
       <c r="I20" s="3">
         <v>16.758645131892056</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="6">
         <v>14.931549971052648</v>
       </c>
       <c r="K20" s="3">
@@ -1790,7 +1800,7 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+      <c r="J21" s="6"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
@@ -1824,7 +1834,7 @@
       <c r="I23" s="3">
         <v>31.643371723844314</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="6">
         <v>0</v>
       </c>
       <c r="K23" s="3">
@@ -1868,7 +1878,7 @@
       <c r="I24" s="3">
         <v>0</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24" s="6">
         <v>0</v>
       </c>
       <c r="K24" s="3">
@@ -1912,7 +1922,7 @@
       <c r="I25" s="3">
         <v>3.0341505792001975</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="6">
         <v>0</v>
       </c>
       <c r="K25" s="3">
@@ -1956,7 +1966,7 @@
       <c r="I26" s="3">
         <v>6.24660677069651</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="6">
         <v>0</v>
       </c>
       <c r="K26" s="3">
@@ -2000,7 +2010,7 @@
       <c r="I27" s="3">
         <v>26.420952619973832</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27" s="6">
         <v>0</v>
       </c>
       <c r="K27" s="3">
@@ -2044,7 +2054,7 @@
       <c r="I28" s="3">
         <v>4.4360155332791473</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28" s="6">
         <v>0</v>
       </c>
       <c r="K28" s="3">
@@ -2088,7 +2098,7 @@
       <c r="I29" s="3">
         <v>12.018493564425444</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29" s="6">
         <v>0</v>
       </c>
       <c r="K29" s="3">
@@ -2132,7 +2142,7 @@
       <c r="I30" s="3">
         <v>1.0115491482392209</v>
       </c>
-      <c r="J30" s="3">
+      <c r="J30" s="6">
         <v>0</v>
       </c>
       <c r="K30" s="3">
@@ -2176,7 +2186,7 @@
       <c r="I31" s="3">
         <v>1.861090599091067E-2</v>
       </c>
-      <c r="J31" s="3">
+      <c r="J31" s="6">
         <v>0</v>
       </c>
       <c r="K31" s="3">
@@ -2220,7 +2230,7 @@
       <c r="I32" s="3">
         <v>20.289787178928979</v>
       </c>
-      <c r="J32" s="3">
+      <c r="J32" s="6">
         <v>0</v>
       </c>
       <c r="K32" s="3">
@@ -2264,7 +2274,7 @@
       <c r="I33" s="3">
         <v>8.4348351906013601</v>
       </c>
-      <c r="J33" s="3">
+      <c r="J33" s="6">
         <v>0</v>
       </c>
       <c r="K33" s="3">
@@ -2308,7 +2318,7 @@
       <c r="I34" s="3">
         <v>4.8791233399540452</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J34" s="6">
         <v>0</v>
       </c>
       <c r="K34" s="3">
@@ -2352,7 +2362,7 @@
       <c r="I35" s="3">
         <v>17.515490403506124</v>
       </c>
-      <c r="J35" s="3">
+      <c r="J35" s="6">
         <v>0</v>
       </c>
       <c r="K35" s="3">
@@ -2396,7 +2406,7 @@
       <c r="I36" s="3">
         <v>14.077528930347164</v>
       </c>
-      <c r="J36" s="3">
+      <c r="J36" s="6">
         <v>0</v>
       </c>
       <c r="K36" s="3">
@@ -2440,7 +2450,7 @@
       <c r="I37" s="3">
         <v>15.829912005767738</v>
       </c>
-      <c r="J37" s="3">
+      <c r="J37" s="6">
         <v>0</v>
       </c>
       <c r="K37" s="3">
@@ -2484,7 +2494,7 @@
       <c r="I38" s="3">
         <v>10.851795655745185</v>
       </c>
-      <c r="J38" s="3">
+      <c r="J38" s="6">
         <v>0</v>
       </c>
       <c r="K38" s="3">
@@ -2528,7 +2538,7 @@
       <c r="I39" s="3">
         <v>11.149122439472846</v>
       </c>
-      <c r="J39" s="3">
+      <c r="J39" s="6">
         <v>0</v>
       </c>
       <c r="K39" s="3">
@@ -2572,7 +2582,7 @@
       <c r="I40" s="3">
         <v>19.27171337382471</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J40" s="6">
         <v>0</v>
       </c>
       <c r="K40" s="3">
@@ -2616,7 +2626,7 @@
       <c r="I41" s="3">
         <v>24.943128178396154</v>
       </c>
-      <c r="J41" s="3">
+      <c r="J41" s="6">
         <v>0</v>
       </c>
       <c r="K41" s="3">
@@ -2660,7 +2670,7 @@
       <c r="I42" s="3">
         <v>25.300359845248689</v>
       </c>
-      <c r="J42" s="3">
+      <c r="J42" s="6">
         <v>0</v>
       </c>
       <c r="K42" s="3">
@@ -2704,7 +2714,7 @@
       <c r="I43" s="3">
         <v>2.2439152648103566</v>
       </c>
-      <c r="J43" s="3">
+      <c r="J43" s="6">
         <v>0</v>
       </c>
       <c r="K43" s="3">
@@ -2748,7 +2758,7 @@
       <c r="I44" s="3">
         <v>4.609974180583289</v>
       </c>
-      <c r="J44" s="3">
+      <c r="J44" s="6">
         <v>0</v>
       </c>
       <c r="K44" s="3">
@@ -2792,7 +2802,7 @@
       <c r="I45" s="3">
         <v>2.7495581195092917</v>
       </c>
-      <c r="J45" s="3">
+      <c r="J45" s="6">
         <v>0</v>
       </c>
       <c r="K45" s="3">
@@ -2836,7 +2846,7 @@
       <c r="I46" s="3">
         <v>4.6696458321083476</v>
       </c>
-      <c r="J46" s="3">
+      <c r="J46" s="6">
         <v>0</v>
       </c>
       <c r="K46" s="3">
@@ -2880,7 +2890,7 @@
       <c r="I47" s="3">
         <v>5.2962361871754906</v>
       </c>
-      <c r="J47" s="3">
+      <c r="J47" s="6">
         <v>0</v>
       </c>
       <c r="K47" s="3">
@@ -2924,7 +2934,7 @@
       <c r="I48" s="3">
         <v>4.893906693586441</v>
       </c>
-      <c r="J48" s="3">
+      <c r="J48" s="6">
         <v>0</v>
       </c>
       <c r="K48" s="3">
@@ -2968,7 +2978,7 @@
       <c r="I49" s="3">
         <v>8.8493852898390575</v>
       </c>
-      <c r="J49" s="3">
+      <c r="J49" s="6">
         <v>0</v>
       </c>
       <c r="K49" s="3">
@@ -3012,7 +3022,7 @@
       <c r="I50" s="3">
         <v>3.5734478439792459</v>
       </c>
-      <c r="J50" s="3">
+      <c r="J50" s="6">
         <v>0</v>
       </c>
       <c r="K50" s="3">
@@ -3056,7 +3066,7 @@
       <c r="I51" s="3">
         <v>16.535708049589662</v>
       </c>
-      <c r="J51" s="3">
+      <c r="J51" s="6">
         <v>0.13968919154880385</v>
       </c>
       <c r="K51" s="3">

</xml_diff>